<commit_message>
start N64 scooby doo
</commit_message>
<xml_diff>
--- a/ScoobyDoo/FrameCompare.xlsx
+++ b/ScoobyDoo/FrameCompare.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repos\adelikat-tas\ScoobyDoo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{738CA835-7F3D-4987-84D0-4A4B404C722E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B8D805F-56F2-46CA-9043-329DCC5113FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="42225" yWindow="435" windowWidth="14490" windowHeight="10890" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="34950" yWindow="2235" windowWidth="14490" windowHeight="10890" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="V4" sheetId="11" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="29">
   <si>
     <t>Place</t>
   </si>
@@ -109,6 +109,15 @@
   </si>
   <si>
     <t>Level appears</t>
+  </si>
+  <si>
+    <t>Get to truck</t>
+  </si>
+  <si>
+    <t>Up ladder</t>
+  </si>
+  <si>
+    <t>Museum appears</t>
   </si>
 </sst>
 </file>
@@ -612,7 +621,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B3" sqref="B3"/>
+      <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -653,23 +662,46 @@
       <c r="F2" s="2"/>
     </row>
     <row r="3" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A3" s="14"/>
+      <c r="A3" s="15" t="s">
+        <v>26</v>
+      </c>
       <c r="B3" s="2"/>
-      <c r="C3" s="2"/>
-      <c r="D3" s="3"/>
+      <c r="C3" s="2">
+        <v>1019</v>
+      </c>
+      <c r="D3" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
       <c r="F3" s="2"/>
     </row>
     <row r="4" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A4" s="14"/>
-      <c r="B4" s="2"/>
+      <c r="A4" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="B4" s="2">
+        <v>1926</v>
+      </c>
       <c r="C4" s="2"/>
-      <c r="D4" s="3"/>
+      <c r="D4" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
     </row>
     <row r="5" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A5" s="14"/>
-      <c r="B5" s="2"/>
-      <c r="C5" s="2"/>
-      <c r="D5" s="3"/>
+      <c r="A5" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="B5" s="2">
+        <v>1976</v>
+      </c>
+      <c r="C5" s="2">
+        <v>1912</v>
+      </c>
+      <c r="D5" s="3">
+        <f t="shared" si="0"/>
+        <v>-64</v>
+      </c>
     </row>
     <row r="6" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A6" s="14"/>

</xml_diff>